<commit_message>
Added '10x Genomics' in the acquisition instrument vendor
Closes #57
</commit_message>
<xml_diff>
--- a/xenium/latest/xenium.xlsx
+++ b/xenium/latest/xenium.xlsx
@@ -271,7 +271,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="331">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -696,6 +696,12 @@
     <t>https://identifiers.org/RRID:SCR_023603</t>
   </si>
   <si>
+    <t>10x Genomics</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023672</t>
+  </si>
+  <si>
     <t>NanoString</t>
   </si>
   <si>
@@ -1251,7 +1257,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-10-17T13:02:56-07:00</t>
+    <t>2024-11-06T10:12:16-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1422,82 +1428,82 @@
         <v>110</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="AD1" t="s" s="1">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="AE1" t="s" s="1">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="AF1" t="s" s="1">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="AG1" t="s" s="1">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="2">
@@ -1505,7 +1511,7 @@
         <v>18</v>
       </c>
       <c r="AG2" t="s" s="34">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
   </sheetData>
@@ -1520,7 +1526,7 @@
       <formula1>'is_targeted'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_vendor'!$A$1:$A$22</formula1>
+      <formula1>'acquisition_instrument_vendor'!$A$1:$A$23</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'acquisition_instrument_model'!$A$1:$A$52</formula1>
@@ -1602,10 +1608,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -1623,10 +1629,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -1644,18 +1650,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -1673,90 +1679,90 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>
@@ -1803,16 +1809,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>327</v>
+        <v>329</v>
       </c>
     </row>
     <row r="2">
@@ -1820,13 +1826,13 @@
         <v>18</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -2293,7 +2299,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2473,6 +2479,14 @@
       </c>
       <c r="B22" t="s" s="0">
         <v>154</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="0">
+        <v>155</v>
+      </c>
+      <c r="B23" t="s" s="0">
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -2490,418 +2504,418 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>
@@ -2919,42 +2933,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -2972,26 +2986,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -3009,18 +3023,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a new oligo panel
Closes #60
</commit_message>
<xml_diff>
--- a/xenium/latest/xenium.xlsx
+++ b/xenium/latest/xenium.xlsx
@@ -271,7 +271,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="335">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -1161,24 +1161,60 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000364</t>
   </si>
   <si>
+    <t>10x Genomics; Chromium Next GEM Single Cell Fixed RNA Mouse Transcriptome Probe Kit, 64 rxns; PN 1000492</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000393</t>
+  </si>
+  <si>
+    <t>10x Genomics; Visium Human Transcriptome Probe Kit-Large; PN 1000364</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000383</t>
+  </si>
+  <si>
+    <t>10x Genomics; Visium Human Transcriptome Probe Kit-Small; PN 1000363</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000326</t>
+  </si>
+  <si>
+    <t>Custom</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C65167</t>
+  </si>
+  <si>
+    <t>NanoString Technologies; GeoMx Human Whole Transcriptome Atlas, 4 slides; PN GMX-RNA-NGS-HuWTA-4</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000363</t>
+  </si>
+  <si>
+    <t>10x Genomics; Chromium Fixed RNA Kit, Human Transcriptome 4 rxns x 4 BC; PN 1000475</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000307</t>
+  </si>
+  <si>
+    <t>10x Genomics; Visium Human Transcriptome Probe Kit v2 - Small; PN 1000466</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000274</t>
+  </si>
+  <si>
+    <t>10x Genomics; Xenium Human Multi-Tissue and Cancer Panel v1; PN 1000626</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000395</t>
+  </si>
+  <si>
     <t>10X Genomics; Chromium Next GEM Single Cell Fixed RNA Human Transcriptome Probe Kit, 64 rxns; PN 1000456</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000376</t>
   </si>
   <si>
-    <t>10x Genomics; Visium Human Transcriptome Probe Kit-Large; PN 1000364</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000383</t>
-  </si>
-  <si>
-    <t>10x Genomics; Visium Human Transcriptome Probe Kit-Small; PN 1000363</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000326</t>
-  </si>
-  <si>
     <t>10x Genomics; Chromium Fixed RNA Kit, Human Transcriptome, 4 rxns x 1 BC; PN 1000474</t>
   </si>
   <si>
@@ -1191,30 +1227,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000362</t>
   </si>
   <si>
-    <t>Custom</t>
-  </si>
-  <si>
-    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C65167</t>
-  </si>
-  <si>
-    <t>NanoString Technologies; GeoMx Human Whole Transcriptome Atlas, 4 slides; PN GMX-RNA-NGS-HuWTA-4</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000363</t>
-  </si>
-  <si>
-    <t>10x Genomics; Chromium Fixed RNA Kit, Human Transcriptome 4 rxns x 4 BC; PN 1000475</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000307</t>
-  </si>
-  <si>
-    <t>10x Genomics; Visium Human Transcriptome Probe Kit v2 - Small; PN 1000466</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000274</t>
-  </si>
-  <si>
     <t>10X Genomics; Chromium Next GEM Single Cell Fixed RNA Human Transcriptome Probe Kit, 16 rxns; PN 1000420</t>
   </si>
   <si>
@@ -1257,7 +1269,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-11-06T10:12:16-08:00</t>
+    <t>2024-12-06T17:11:10-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1485,25 +1497,25 @@
         <v>293</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="AD1" t="s" s="1">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="AE1" t="s" s="1">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="AF1" t="s" s="1">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="AG1" t="s" s="1">
-        <v>322</v>
+        <v>326</v>
       </c>
     </row>
     <row r="2">
@@ -1511,7 +1523,7 @@
         <v>18</v>
       </c>
       <c r="AG2" t="s" s="34">
-        <v>323</v>
+        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -1582,7 +1594,7 @@
       <formula1>'probe_hybridization_time_unit'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="Z2:Z1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'oligo_probe_panel'!$A$1:$A$11</formula1>
+      <formula1>'oligo_probe_panel'!$A$1:$A$13</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AA2:AA1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'is_custom_probes_used'!$A$1:$A$2</formula1>
@@ -1671,7 +1683,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1763,6 +1775,22 @@
       </c>
       <c r="B11" t="s" s="0">
         <v>315</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>316</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>318</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>319</v>
       </c>
     </row>
   </sheetData>
@@ -1809,16 +1837,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>329</v>
+        <v>333</v>
       </c>
     </row>
     <row r="2">
@@ -1826,13 +1854,13 @@
         <v>18</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>330</v>
+        <v>334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new oligo panels
Closes #106, #107
</commit_message>
<xml_diff>
--- a/xenium/latest/xenium.xlsx
+++ b/xenium/latest/xenium.xlsx
@@ -271,7 +271,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="431">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -1455,12 +1455,30 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000395</t>
   </si>
   <si>
+    <t>10x Genomics; Xenium Custom Gene Expression Panel (up to 50 genes); PN 1000464</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000445</t>
+  </si>
+  <si>
+    <t>10x Genomics; Xenium Custom Gene Expression Panel (51-100 genes); PN 1000561</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000444</t>
+  </si>
+  <si>
     <t>10X Genomics; Chromium Next GEM Single Cell Fixed RNA Human Transcriptome Probe Kit, 64 rxns; PN 1000456</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000376</t>
   </si>
   <si>
+    <t>10x Genomics; Xenium Human Colon Gene Expression Panel; PN 1000642</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000446</t>
+  </si>
+  <si>
     <t>NanoString Technologies; CosMx Human Immuno-Oncology Panel (Protein, 64 Plex); PN CMX-H-IOP-64P-P</t>
   </si>
   <si>
@@ -1479,6 +1497,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000362</t>
   </si>
   <si>
+    <t>10x Genomics; Xenium Human Lung Gene Expression Panel; PN 1000601</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000443</t>
+  </si>
+  <si>
     <t>NanoString Technologies; CosMx Human Universal Cell Characterization Panel (RNA, 1000 Plex); PN CMX-H-USCP-1KP-R</t>
   </si>
   <si>
@@ -1533,7 +1557,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-07-16T10:38:03-07:00</t>
+    <t>2025-07-21T13:59:19-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1761,25 +1785,25 @@
         <v>369</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>408</v>
+        <v>416</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>409</v>
+        <v>417</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>410</v>
+        <v>418</v>
       </c>
       <c r="AD1" t="s" s="1">
-        <v>411</v>
+        <v>419</v>
       </c>
       <c r="AE1" t="s" s="1">
-        <v>412</v>
+        <v>420</v>
       </c>
       <c r="AF1" t="s" s="1">
-        <v>413</v>
+        <v>421</v>
       </c>
       <c r="AG1" t="s" s="1">
-        <v>414</v>
+        <v>422</v>
       </c>
     </row>
     <row r="2">
@@ -1787,7 +1811,7 @@
         <v>22</v>
       </c>
       <c r="AG2" t="s" s="34">
-        <v>415</v>
+        <v>423</v>
       </c>
     </row>
   </sheetData>
@@ -1858,7 +1882,7 @@
       <formula1>'probe_hybridization_time_unit'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="Z2:Z1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'oligo_probe_panel'!$A$1:$A$19</formula1>
+      <formula1>'oligo_probe_panel'!$A$1:$A$23</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AA2:AA1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'is_custom_probes_used'!$A$1:$A$2</formula1>
@@ -1947,7 +1971,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2103,6 +2127,38 @@
       </c>
       <c r="B19" t="s" s="0">
         <v>407</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="0">
+        <v>408</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="0">
+        <v>410</v>
+      </c>
+      <c r="B21" t="s" s="0">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="0">
+        <v>412</v>
+      </c>
+      <c r="B22" t="s" s="0">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="0">
+        <v>414</v>
+      </c>
+      <c r="B23" t="s" s="0">
+        <v>415</v>
       </c>
     </row>
   </sheetData>
@@ -2149,16 +2205,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>416</v>
+        <v>424</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>417</v>
+        <v>425</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>419</v>
+        <v>427</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>421</v>
+        <v>429</v>
       </c>
     </row>
     <row r="2">
@@ -2166,13 +2222,13 @@
         <v>22</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>418</v>
+        <v>426</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>420</v>
+        <v>428</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>422</v>
+        <v>430</v>
       </c>
     </row>
   </sheetData>

</xml_diff>